<commit_message>
import and export grade for an assignment
</commit_message>
<xml_diff>
--- a/xlsxFolder/studentList.xlsx
+++ b/xlsxFolder/studentList.xlsx
@@ -1,53 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DinhKhoi\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B0F476-8489-4D4A-B098-7C3BDB416B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="2628" yWindow="3540" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
     <sheet name="studentList.xlsx" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>studentId</t>
-  </si>
-  <si>
-    <t>fullname</t>
-  </si>
-  <si>
-    <t>27060343</t>
-  </si>
-  <si>
-    <t>Nguyễn Đình Khôi</t>
-  </si>
-  <si>
-    <t>1233333</t>
-  </si>
-  <si>
-    <t>Yến Trâm</t>
-  </si>
-  <si>
-    <t>Ngân Trâm</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
+  <numFmts count="1">
+    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -80,18 +46,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -416,52 +374,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>studentId</v>
+      </c>
+      <c r="B1" t="str">
+        <v>fullname</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>27060343</v>
+      </c>
+      <c r="B2" t="str">
+        <v>Nguyễn Đình Khôi</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>1233333</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Yến Trâm</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" t="str">
         <v>18120042</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B4" t="str">
+        <v>Ngân Trâm</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B3" numberStoredAsText="1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>